<commit_message>
Added 34 java projects from github
</commit_message>
<xml_diff>
--- a/data_gathering/program_list.xlsx
+++ b/data_gathering/program_list.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyson\Documents\seng300Group3\data_gathering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Documents\seng300Group3\data_gathering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EC0C8E-9CC0-4ECA-8F35-81E6C711089F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{B4B9B83D-8048-4FD0-923E-D4ADBE9CB099}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>Link</t>
   </si>
@@ -37,13 +36,226 @@
   </si>
   <si>
     <t>Example program name</t>
+  </si>
+  <si>
+    <t>Commiter</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>ZXing ("Zebra Crossing")</t>
+  </si>
+  <si>
+    <t>https://github.com/zxing/zxing</t>
+  </si>
+  <si>
+    <t>Tyson</t>
+  </si>
+  <si>
+    <t>https://github.com/square/leakcanary</t>
+  </si>
+  <si>
+    <t>leakcanary</t>
+  </si>
+  <si>
+    <t>https://github.com/Konloch/bytecode-viewer</t>
+  </si>
+  <si>
+    <t>bytecode viewer</t>
+  </si>
+  <si>
+    <t>https://github.com/orhanobut/logger</t>
+  </si>
+  <si>
+    <t>logger</t>
+  </si>
+  <si>
+    <t>https://github.com/deeplearning4j/deeplearning4j</t>
+  </si>
+  <si>
+    <t>deeplearning4j</t>
+  </si>
+  <si>
+    <t>https://github.com/junit-team/junit4</t>
+  </si>
+  <si>
+    <t>junit4</t>
+  </si>
+  <si>
+    <t>https://github.com/mockito/mockito</t>
+  </si>
+  <si>
+    <t>mockito</t>
+  </si>
+  <si>
+    <t>jooq</t>
+  </si>
+  <si>
+    <t>https://github.com/jOOQ/jOOQ</t>
+  </si>
+  <si>
+    <t>MineCraftForge</t>
+  </si>
+  <si>
+    <t>https://github.com/MinecraftForge/MinecraftForge</t>
+  </si>
+  <si>
+    <t>Cryptomator</t>
+  </si>
+  <si>
+    <t>https://github.com/cryptomator/cryptomator</t>
+  </si>
+  <si>
+    <t>JUnit5</t>
+  </si>
+  <si>
+    <t>https://github.com/junit-team/junit5</t>
+  </si>
+  <si>
+    <t>https://github.com/mongodb/mongo-java-driver</t>
+  </si>
+  <si>
+    <t>mongo java driver</t>
+  </si>
+  <si>
+    <t>reflections</t>
+  </si>
+  <si>
+    <t>https://github.com/ronmamo/reflections</t>
+  </si>
+  <si>
+    <t>NullAway</t>
+  </si>
+  <si>
+    <t>https://github.com/uber/NullAway</t>
+  </si>
+  <si>
+    <t>https://github.com/powermock/powermock</t>
+  </si>
+  <si>
+    <t>powermock</t>
+  </si>
+  <si>
+    <t>https://github.com/CrawlScript/WebCollector</t>
+  </si>
+  <si>
+    <t>WebCollector</t>
+  </si>
+  <si>
+    <t>ninja</t>
+  </si>
+  <si>
+    <t>https://github.com/ninjaframework/ninja</t>
+  </si>
+  <si>
+    <t>jmonkeyengine</t>
+  </si>
+  <si>
+    <t>https://github.com/jMonkeyEngine/jmonkeyengine</t>
+  </si>
+  <si>
+    <t>Shuttle</t>
+  </si>
+  <si>
+    <t>https://github.com/timusus/Shuttle</t>
+  </si>
+  <si>
+    <t>mockserver</t>
+  </si>
+  <si>
+    <t>https://github.com/jamesdbloom/mockserver</t>
+  </si>
+  <si>
+    <t>Minimal Todo</t>
+  </si>
+  <si>
+    <t>https://github.com/avjinder/Minimal-Todo</t>
+  </si>
+  <si>
+    <t>Traccar GPS Tracking</t>
+  </si>
+  <si>
+    <t>https://github.com/traccar/traccar</t>
+  </si>
+  <si>
+    <t>JSqlParser</t>
+  </si>
+  <si>
+    <t>https://github.com/JSQLParser/JSqlParser</t>
+  </si>
+  <si>
+    <t>strman</t>
+  </si>
+  <si>
+    <t>https://github.com/shekhargulati/strman-java</t>
+  </si>
+  <si>
+    <t>Apache Maven</t>
+  </si>
+  <si>
+    <t>https://github.com/apache/maven</t>
+  </si>
+  <si>
+    <t>tablesaw</t>
+  </si>
+  <si>
+    <t>https://github.com/jtablesaw/tablesaw</t>
+  </si>
+  <si>
+    <t>https://github.com/cmusphinx/sphinx4</t>
+  </si>
+  <si>
+    <t>sphinx4</t>
+  </si>
+  <si>
+    <t>jbot</t>
+  </si>
+  <si>
+    <t>https://github.com/ramswaroop/jbot</t>
+  </si>
+  <si>
+    <t>https://github.com/JorenSix/TarsosDSP</t>
+  </si>
+  <si>
+    <t>TarsosDSP</t>
+  </si>
+  <si>
+    <t>lanterna</t>
+  </si>
+  <si>
+    <t>https://github.com/mabe02/lanterna</t>
+  </si>
+  <si>
+    <t>turbo editor</t>
+  </si>
+  <si>
+    <t>https://github.com/vmihalachi/turbo-editor</t>
+  </si>
+  <si>
+    <t>visualvm</t>
+  </si>
+  <si>
+    <t>https://github.com/oracle/visualvm</t>
+  </si>
+  <si>
+    <t>mycollab</t>
+  </si>
+  <si>
+    <t>https://github.com/MyCollab/mycollab</t>
+  </si>
+  <si>
+    <t>spotbugs</t>
+  </si>
+  <si>
+    <t>https://github.com/spotbugs/spotbugs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,14 +267,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,17 +295,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,43 +616,418 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DD0A52-C986-4942-A170-A5AC0DA1B38F}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.81640625" customWidth="1"/>
-    <col min="2" max="2" width="48.6328125" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="82.5703125" customWidth="1"/>
+    <col min="3" max="3" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" s="1"/>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{4875A586-83B1-4268-AD14-5FA49AB1CBFC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>